<commit_message>
Updated templates for questionnaire, added jobs for experiments.
</commit_message>
<xml_diff>
--- a/AdapQuestBackend/data/templates/adaptive.questionnaire.template.xlsx
+++ b/AdapQuestBackend/data/templates/adaptive.questionnaire.template.xlsx
@@ -5,16 +5,18 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\adaptive\adapquest\AdapQuestBackend\data\surveys\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\adaptive\adapquest\AdapQuestBackend\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD01DE5D-D54B-4F67-94B0-96AEDEE16B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C55119-E18A-4CC7-9AAC-511B33BC686B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
     <sheet name="Questions" sheetId="14" r:id="rId2"/>
+    <sheet name="Profiles" sheetId="15" r:id="rId3"/>
+    <sheet name="Answers" sheetId="16" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="189">
   <si>
     <t>Mandatory</t>
   </si>
@@ -43,15 +45,9 @@
     <t>Questions_Text</t>
   </si>
   <si>
-    <t>Q_ID</t>
-  </si>
-  <si>
     <t>S_ID</t>
   </si>
   <si>
-    <t>Id_Ans</t>
-  </si>
-  <si>
     <t>KO</t>
   </si>
   <si>
@@ -581,13 +577,40 @@
   </si>
   <si>
     <t>Q03A10</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>P3</t>
+  </si>
+  <si>
+    <t>SKILLS</t>
+  </si>
+  <si>
+    <t>Question_ID</t>
+  </si>
+  <si>
+    <t>Answer_ID</t>
+  </si>
+  <si>
+    <t>ANSWER_ID</t>
+  </si>
+  <si>
+    <t>QUESTION_ID</t>
+  </si>
+  <si>
+    <t>Profiles</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -609,6 +632,10 @@
       <sz val="8"/>
       <name val="Arial"/>
       <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="2">
@@ -981,8 +1008,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A944510-FF7A-456D-8D81-52A411BFF42E}">
   <dimension ref="A1:B22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -993,15 +1020,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="B2">
         <v>0.1</v>
@@ -1009,7 +1036,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="B3">
         <v>0.95</v>
@@ -1017,7 +1044,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B4">
         <v>0.05</v>
@@ -1025,29 +1052,29 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B7" s="3"/>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="B8">
         <v>3600</v>
@@ -1055,12 +1082,12 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B10" t="b">
         <v>1</v>
@@ -1068,7 +1095,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B11" t="b">
         <v>0</v>
@@ -1076,7 +1103,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1084,7 +1111,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="B13" t="b">
         <v>1</v>
@@ -1092,7 +1119,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B14" t="b">
         <v>0</v>
@@ -1100,7 +1127,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -1108,7 +1135,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B16">
         <v>1000</v>
@@ -1116,7 +1143,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B17">
         <v>18</v>
@@ -1124,7 +1151,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B18">
         <v>18</v>
@@ -1132,7 +1159,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B19">
         <v>0.1</v>
@@ -1140,7 +1167,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="B20">
         <v>0.25</v>
@@ -1148,7 +1175,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B21">
         <v>1</v>
@@ -1156,7 +1183,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -1172,29 +1199,23 @@
   <dimension ref="A1:X116"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="W8" sqref="W8"/>
+      <selection sqref="A1:X1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.21875" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="16" width="4" bestFit="1" customWidth="1"/>
-    <col min="17" max="24" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="8.88671875" style="1" customWidth="1"/>
+    <col min="6" max="24" width="8.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
       <c r="C1" t="s">
         <v>0</v>
       </c>
@@ -1202,67 +1223,67 @@
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>186</v>
       </c>
       <c r="G1" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="H1" s="3"/>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.2">
       <c r="H2" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="N2" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="O2" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="P2" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="Q2" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="R2" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="Q2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>47</v>
-      </c>
-      <c r="W2" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="X2" s="3" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="3" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1276,7 +1297,7 @@
         <v>1</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E3" s="1">
         <v>0</v>
@@ -1285,7 +1306,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="H3">
         <v>0.3</v>
@@ -1348,7 +1369,7 @@
         <v>2</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="H4">
         <v>0.9</v>
@@ -1411,7 +1432,7 @@
         <v>3</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="H5">
         <v>0</v>
@@ -1474,7 +1495,7 @@
         <v>4</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="H6">
         <v>0</v>
@@ -1537,7 +1558,7 @@
         <v>5</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="H7">
         <v>0</v>
@@ -1600,7 +1621,7 @@
         <v>6</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="H8">
         <v>0</v>
@@ -1663,7 +1684,7 @@
         <v>7</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="H9">
         <v>0</v>
@@ -1726,7 +1747,7 @@
         <v>8</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="H10">
         <v>0.3</v>
@@ -1789,7 +1810,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="H11">
         <v>0.9</v>
@@ -1854,7 +1875,7 @@
         <v>1</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="E12" s="1">
         <v>0</v>
@@ -1863,7 +1884,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="H12">
         <v>0.9</v>
@@ -1922,7 +1943,7 @@
         <v>2</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="H13">
         <v>0.6</v>
@@ -1981,7 +2002,7 @@
         <v>3</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="H14">
         <v>0</v>
@@ -2040,7 +2061,7 @@
         <v>4</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="H15">
         <v>0.6</v>
@@ -2105,7 +2126,7 @@
         <v>0</v>
       </c>
       <c r="D16" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E16" s="1">
         <v>1</v>
@@ -2114,7 +2135,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H16">
         <v>0</v>
@@ -2173,7 +2194,7 @@
         <v>2</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="H17">
         <v>0.3</v>
@@ -2232,7 +2253,7 @@
         <v>3</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H18">
         <v>0</v>
@@ -2291,7 +2312,7 @@
         <v>4</v>
       </c>
       <c r="G19" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -2350,7 +2371,7 @@
         <v>5</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="H20">
         <v>0</v>
@@ -2409,7 +2430,7 @@
         <v>6</v>
       </c>
       <c r="G21" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="H21">
         <v>0.3</v>
@@ -2468,7 +2489,7 @@
         <v>7</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="H22">
         <v>0.6</v>
@@ -2527,7 +2548,7 @@
         <v>8</v>
       </c>
       <c r="G23" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="H23">
         <v>0</v>
@@ -2586,7 +2607,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="H24">
         <v>0</v>
@@ -2645,7 +2666,7 @@
         <v>10</v>
       </c>
       <c r="G25" s="3" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="H25">
         <v>0.3</v>
@@ -2663,7 +2684,7 @@
         <v>0.3</v>
       </c>
       <c r="M25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N25">
         <v>0.3</v>
@@ -2684,7 +2705,7 @@
         <v>0.3</v>
       </c>
       <c r="T25" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U25">
         <v>0.3</v>
@@ -2710,7 +2731,7 @@
         <v>0</v>
       </c>
       <c r="D26" s="1" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E26" s="1">
         <v>1</v>
@@ -2719,7 +2740,7 @@
         <v>1</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="H26">
         <v>0</v>
@@ -2778,7 +2799,7 @@
         <v>2</v>
       </c>
       <c r="G27" s="3" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="H27">
         <v>0</v>
@@ -2837,7 +2858,7 @@
         <v>3</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="H28">
         <v>0.3</v>
@@ -2849,16 +2870,16 @@
         <v>0.3</v>
       </c>
       <c r="K28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O28">
         <v>0.3</v>
@@ -2888,7 +2909,7 @@
         <v>0.3</v>
       </c>
       <c r="X28" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:24" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2902,7 +2923,7 @@
         <v>0</v>
       </c>
       <c r="D29" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E29" s="1">
         <v>1</v>
@@ -2911,7 +2932,7 @@
         <v>1</v>
       </c>
       <c r="G29" s="4" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="H29">
         <v>0</v>
@@ -2970,7 +2991,7 @@
         <v>2</v>
       </c>
       <c r="G30" s="4" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="H30">
         <v>0.9</v>
@@ -3029,7 +3050,7 @@
         <v>3</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="H31">
         <v>0</v>
@@ -3088,7 +3109,7 @@
         <v>4</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="H32">
         <v>0</v>
@@ -3100,16 +3121,16 @@
         <v>0.3</v>
       </c>
       <c r="K32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="L32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="M32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N32" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="O32">
         <v>0.3</v>
@@ -3153,7 +3174,7 @@
         <v>0</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E33" s="1">
         <v>1</v>
@@ -3162,7 +3183,7 @@
         <v>1</v>
       </c>
       <c r="G33" s="3" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H33">
         <v>0</v>
@@ -3221,7 +3242,7 @@
         <v>2</v>
       </c>
       <c r="G34" s="3" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="H34">
         <v>0</v>
@@ -3280,7 +3301,7 @@
         <v>3</v>
       </c>
       <c r="G35" s="3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H35">
         <v>0</v>
@@ -3339,7 +3360,7 @@
         <v>4</v>
       </c>
       <c r="G36" s="3" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="H36">
         <v>0</v>
@@ -3398,7 +3419,7 @@
         <v>5</v>
       </c>
       <c r="G37" s="3" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="H37">
         <v>0</v>
@@ -3457,7 +3478,7 @@
         <v>6</v>
       </c>
       <c r="G38" s="3" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H38">
         <v>0</v>
@@ -3516,7 +3537,7 @@
         <v>7</v>
       </c>
       <c r="G39" s="3" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="H39">
         <v>0</v>
@@ -3575,13 +3596,13 @@
         <v>8</v>
       </c>
       <c r="G40" s="3" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="H40">
         <v>0.3</v>
       </c>
       <c r="I40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J40">
         <v>0</v>
@@ -3599,16 +3620,16 @@
         <v>0</v>
       </c>
       <c r="O40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="P40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="Q40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="R40" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S40">
         <v>0.3</v>
@@ -3640,7 +3661,7 @@
         <v>0</v>
       </c>
       <c r="D41" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E41" s="1">
         <v>1</v>
@@ -3649,7 +3670,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="3" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="H41">
         <v>0</v>
@@ -3708,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="G42" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="H42">
         <v>0</v>
@@ -3767,7 +3788,7 @@
         <v>3</v>
       </c>
       <c r="G43" s="3" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="H43">
         <v>0</v>
@@ -3826,7 +3847,7 @@
         <v>4</v>
       </c>
       <c r="G44" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="H44">
         <v>0</v>
@@ -3885,7 +3906,7 @@
         <v>5</v>
       </c>
       <c r="G45" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="H45">
         <v>0.3</v>
@@ -3921,7 +3942,7 @@
         <v>0.3</v>
       </c>
       <c r="S45" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="T45">
         <v>0.3</v>
@@ -3950,7 +3971,7 @@
         <v>0</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E46" s="1">
         <v>1</v>
@@ -3959,7 +3980,7 @@
         <v>1</v>
       </c>
       <c r="G46" s="3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="H46">
         <v>0.6</v>
@@ -4018,7 +4039,7 @@
         <v>2</v>
       </c>
       <c r="G47" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="H47">
         <v>0</v>
@@ -4077,7 +4098,7 @@
         <v>3</v>
       </c>
       <c r="G48" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="H48">
         <v>0.3</v>
@@ -4136,7 +4157,7 @@
         <v>4</v>
       </c>
       <c r="G49" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="H49">
         <v>0.3</v>
@@ -4195,7 +4216,7 @@
         <v>5</v>
       </c>
       <c r="G50" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H50">
         <v>0.3</v>
@@ -4234,16 +4255,16 @@
         <v>0.3</v>
       </c>
       <c r="T50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="V50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="W50" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="X50">
         <v>0.3</v>
@@ -4260,7 +4281,7 @@
         <v>0</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E51" s="1">
         <v>1</v>
@@ -4269,7 +4290,7 @@
         <v>1</v>
       </c>
       <c r="G51" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="H51">
         <v>0.6</v>
@@ -4328,7 +4349,7 @@
         <v>2</v>
       </c>
       <c r="G52" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="H52">
         <v>0.3</v>
@@ -4387,7 +4408,7 @@
         <v>3</v>
       </c>
       <c r="G53" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="H53">
         <v>0</v>
@@ -4446,7 +4467,7 @@
         <v>4</v>
       </c>
       <c r="G54" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="H54">
         <v>0.3</v>
@@ -4505,7 +4526,7 @@
         <v>5</v>
       </c>
       <c r="G55" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="H55">
         <v>0</v>
@@ -4564,7 +4585,7 @@
         <v>6</v>
       </c>
       <c r="G56" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="H56">
         <v>0.6</v>
@@ -4623,7 +4644,7 @@
         <v>7</v>
       </c>
       <c r="G57" s="3" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="H57">
         <v>0</v>
@@ -4662,7 +4683,7 @@
         <v>0.3</v>
       </c>
       <c r="T57" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U57">
         <v>0</v>
@@ -4688,7 +4709,7 @@
         <v>0</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E58" s="1">
         <v>1</v>
@@ -4697,7 +4718,7 @@
         <v>1</v>
       </c>
       <c r="G58" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="H58">
         <v>0</v>
@@ -4756,7 +4777,7 @@
         <v>2</v>
       </c>
       <c r="G59" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="H59">
         <v>0</v>
@@ -4815,7 +4836,7 @@
         <v>3</v>
       </c>
       <c r="G60" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="H60">
         <v>0</v>
@@ -4874,7 +4895,7 @@
         <v>4</v>
       </c>
       <c r="G61" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H61">
         <v>0</v>
@@ -4933,7 +4954,7 @@
         <v>5</v>
       </c>
       <c r="G62" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="H62">
         <v>0</v>
@@ -4992,7 +5013,7 @@
         <v>6</v>
       </c>
       <c r="G63" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H63">
         <v>0</v>
@@ -5051,16 +5072,16 @@
         <v>7</v>
       </c>
       <c r="G64" s="3" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="H64">
         <v>0.3</v>
       </c>
       <c r="I64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="J64" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="K64">
         <v>0.3</v>
@@ -5116,7 +5137,7 @@
         <v>0</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="E65" s="1">
         <v>1</v>
@@ -5125,7 +5146,7 @@
         <v>1</v>
       </c>
       <c r="G65" s="3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="H65">
         <v>0</v>
@@ -5184,7 +5205,7 @@
         <v>2</v>
       </c>
       <c r="G66" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="H66">
         <v>0</v>
@@ -5243,7 +5264,7 @@
         <v>3</v>
       </c>
       <c r="G67" s="3" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="H67">
         <v>0</v>
@@ -5302,7 +5323,7 @@
         <v>4</v>
       </c>
       <c r="G68" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H68">
         <v>0</v>
@@ -5361,7 +5382,7 @@
         <v>5</v>
       </c>
       <c r="G69" s="3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H69">
         <v>0</v>
@@ -5420,7 +5441,7 @@
         <v>6</v>
       </c>
       <c r="G70" s="3" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="H70">
         <v>0.3</v>
@@ -5485,7 +5506,7 @@
         <v>0</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="E71" s="1">
         <v>1</v>
@@ -5494,7 +5515,7 @@
         <v>1</v>
       </c>
       <c r="G71" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H71">
         <v>0.6</v>
@@ -5553,7 +5574,7 @@
         <v>2</v>
       </c>
       <c r="G72" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H72">
         <v>0.6</v>
@@ -5612,7 +5633,7 @@
         <v>3</v>
       </c>
       <c r="G73" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H73">
         <v>0.3</v>
@@ -5645,7 +5666,7 @@
         <v>0.3</v>
       </c>
       <c r="R73" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="S73">
         <v>0.3</v>
@@ -5677,7 +5698,7 @@
         <v>0</v>
       </c>
       <c r="D74" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E74" s="1">
         <v>1</v>
@@ -5686,7 +5707,7 @@
         <v>1</v>
       </c>
       <c r="G74" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H74">
         <v>0</v>
@@ -5745,7 +5766,7 @@
         <v>2</v>
       </c>
       <c r="G75" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H75">
         <v>0</v>
@@ -5804,7 +5825,7 @@
         <v>3</v>
       </c>
       <c r="G76" s="3" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="H76">
         <v>0.3</v>
@@ -5822,7 +5843,7 @@
         <v>0</v>
       </c>
       <c r="M76" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="N76">
         <v>0</v>
@@ -5869,7 +5890,7 @@
         <v>0</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="E77" s="1">
         <v>1</v>
@@ -5878,7 +5899,7 @@
         <v>1</v>
       </c>
       <c r="G77" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H77">
         <v>0</v>
@@ -5937,7 +5958,7 @@
         <v>2</v>
       </c>
       <c r="G78" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="H78">
         <v>0</v>
@@ -5996,7 +6017,7 @@
         <v>3</v>
       </c>
       <c r="G79" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="H79">
         <v>0</v>
@@ -6055,7 +6076,7 @@
         <v>4</v>
       </c>
       <c r="G80" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H80">
         <v>0.9</v>
@@ -6114,7 +6135,7 @@
         <v>5</v>
       </c>
       <c r="G81" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="H81">
         <v>0</v>
@@ -6173,7 +6194,7 @@
         <v>6</v>
       </c>
       <c r="G82" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H82">
         <v>0</v>
@@ -6232,7 +6253,7 @@
         <v>7</v>
       </c>
       <c r="G83" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="H83">
         <v>0</v>
@@ -6291,7 +6312,7 @@
         <v>8</v>
       </c>
       <c r="G84" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="H84">
         <v>0</v>
@@ -6350,7 +6371,7 @@
         <v>9</v>
       </c>
       <c r="G85" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="H85">
         <v>0</v>
@@ -6409,7 +6430,7 @@
         <v>10</v>
       </c>
       <c r="G86" s="3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H86">
         <v>0</v>
@@ -6468,7 +6489,7 @@
         <v>11</v>
       </c>
       <c r="G87" s="3" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="H87">
         <v>0</v>
@@ -6527,7 +6548,7 @@
         <v>12</v>
       </c>
       <c r="G88" s="3" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="H88">
         <v>0</v>
@@ -6586,7 +6607,7 @@
         <v>13</v>
       </c>
       <c r="G89" s="3" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="H89">
         <v>0</v>
@@ -6645,7 +6666,7 @@
         <v>14</v>
       </c>
       <c r="G90" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="H90">
         <v>0</v>
@@ -6710,7 +6731,7 @@
         <v>0</v>
       </c>
       <c r="D91" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E91" s="1">
         <v>1</v>
@@ -6719,7 +6740,7 @@
         <v>1</v>
       </c>
       <c r="G91" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="H91">
         <v>0</v>
@@ -6778,7 +6799,7 @@
         <v>2</v>
       </c>
       <c r="G92" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="H92">
         <v>0</v>
@@ -6837,7 +6858,7 @@
         <v>3</v>
       </c>
       <c r="G93" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="H93">
         <v>0</v>
@@ -6896,7 +6917,7 @@
         <v>4</v>
       </c>
       <c r="G94" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="H94">
         <v>0</v>
@@ -6955,7 +6976,7 @@
         <v>5</v>
       </c>
       <c r="G95" s="3" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="H95">
         <v>0.3</v>
@@ -6994,7 +7015,7 @@
         <v>0.3</v>
       </c>
       <c r="T95" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="U95">
         <v>0</v>
@@ -7020,7 +7041,7 @@
         <v>0</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E96" s="1">
         <v>1</v>
@@ -7029,7 +7050,7 @@
         <v>1</v>
       </c>
       <c r="G96" s="3" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="H96">
         <v>0</v>
@@ -7088,7 +7109,7 @@
         <v>2</v>
       </c>
       <c r="G97" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="H97">
         <v>0</v>
@@ -7147,7 +7168,7 @@
         <v>3</v>
       </c>
       <c r="G98" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="H98">
         <v>0</v>
@@ -7206,7 +7227,7 @@
         <v>4</v>
       </c>
       <c r="G99" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="H99">
         <v>0</v>
@@ -7265,7 +7286,7 @@
         <v>5</v>
       </c>
       <c r="G100" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="H100">
         <v>0.6</v>
@@ -7324,7 +7345,7 @@
         <v>6</v>
       </c>
       <c r="G101" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="H101">
         <v>0.3</v>
@@ -7389,7 +7410,7 @@
         <v>0</v>
       </c>
       <c r="D102" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E102" s="1">
         <v>1</v>
@@ -7398,7 +7419,7 @@
         <v>1</v>
       </c>
       <c r="G102" s="3" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="H102">
         <v>0</v>
@@ -7457,7 +7478,7 @@
         <v>2</v>
       </c>
       <c r="G103" s="3" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="H103">
         <v>0</v>
@@ -7516,7 +7537,7 @@
         <v>3</v>
       </c>
       <c r="G104" s="3" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="H104">
         <v>0</v>
@@ -7575,7 +7596,7 @@
         <v>4</v>
       </c>
       <c r="G105" s="3" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H105">
         <v>0</v>
@@ -7634,7 +7655,7 @@
         <v>5</v>
       </c>
       <c r="G106" s="3" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="H106">
         <v>0</v>
@@ -7693,7 +7714,7 @@
         <v>6</v>
       </c>
       <c r="G107" s="3" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="H107">
         <v>0.3</v>
@@ -7758,7 +7779,7 @@
         <v>0</v>
       </c>
       <c r="D108" s="1" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E108" s="1">
         <v>1</v>
@@ -7767,7 +7788,7 @@
         <v>1</v>
       </c>
       <c r="G108" s="3" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="H108">
         <v>0.9</v>
@@ -7826,7 +7847,7 @@
         <v>2</v>
       </c>
       <c r="G109" s="3" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="H109">
         <v>0.9</v>
@@ -7885,7 +7906,7 @@
         <v>3</v>
       </c>
       <c r="G110" s="3" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="H110">
         <v>0.9</v>
@@ -7944,7 +7965,7 @@
         <v>4</v>
       </c>
       <c r="G111" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="H111">
         <v>0.9</v>
@@ -8003,7 +8024,7 @@
         <v>5</v>
       </c>
       <c r="G112" s="3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="H112">
         <v>0.9</v>
@@ -8062,7 +8083,7 @@
         <v>6</v>
       </c>
       <c r="G113" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="H113">
         <v>0.9</v>
@@ -8121,7 +8142,7 @@
         <v>7</v>
       </c>
       <c r="G114" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="H114">
         <v>0.9</v>
@@ -8180,7 +8201,7 @@
         <v>8</v>
       </c>
       <c r="G115" s="3" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="H115">
         <v>0.9</v>
@@ -8239,7 +8260,7 @@
         <v>9</v>
       </c>
       <c r="G116" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="H116">
         <v>0</v>
@@ -8299,13 +8320,2258 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6385A002-8632-45BD-B5D7-4E064A8C1777}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="4" width="8.88671875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D1" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B5">
+        <v>0</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="B9">
+        <v>0</v>
+      </c>
+      <c r="C9">
+        <v>0</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10">
+        <v>1</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A11" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>1</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A12" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="B12">
+        <v>0</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A13" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="B13">
+        <v>1</v>
+      </c>
+      <c r="C13">
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A14" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B14">
+        <v>0</v>
+      </c>
+      <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A15" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B15">
+        <v>0</v>
+      </c>
+      <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A16" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16">
+        <v>0</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A17" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B17">
+        <v>0</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A18" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18">
+        <v>0</v>
+      </c>
+      <c r="C18">
+        <v>1</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="4" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DD315C-5019-4FDD-A7E5-B0550B9F67F5}">
+  <dimension ref="A1:E116"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" t="s">
+        <v>185</v>
+      </c>
+      <c r="C1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>180</v>
+      </c>
+      <c r="D2" t="s">
+        <v>181</v>
+      </c>
+      <c r="E2" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>1</v>
+      </c>
+      <c r="C3">
+        <v>0</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>2</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>5</v>
+      </c>
+      <c r="C7">
+        <v>0</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="1">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>6</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8">
+        <v>0</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="1">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="1">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>8</v>
+      </c>
+      <c r="C10">
+        <v>0</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="1">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>9</v>
+      </c>
+      <c r="C11">
+        <v>0</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>2</v>
+      </c>
+      <c r="B12">
+        <v>1</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13">
+        <v>2</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="1">
+        <v>2</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14">
+        <v>1</v>
+      </c>
+      <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="1">
+        <v>2</v>
+      </c>
+      <c r="B15">
+        <v>4</v>
+      </c>
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>3</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="C16">
+        <v>0</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17">
+        <v>2</v>
+      </c>
+      <c r="C17">
+        <v>0</v>
+      </c>
+      <c r="D17">
+        <v>0</v>
+      </c>
+      <c r="E17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18">
+        <v>3</v>
+      </c>
+      <c r="C18">
+        <v>0</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>4</v>
+      </c>
+      <c r="C19">
+        <v>1</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="1">
+        <v>3</v>
+      </c>
+      <c r="B20">
+        <v>5</v>
+      </c>
+      <c r="C20">
+        <v>0</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A21" s="1">
+        <v>3</v>
+      </c>
+      <c r="B21">
+        <v>6</v>
+      </c>
+      <c r="C21">
+        <v>0</v>
+      </c>
+      <c r="D21">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A22" s="1">
+        <v>3</v>
+      </c>
+      <c r="B22">
+        <v>7</v>
+      </c>
+      <c r="C22">
+        <v>0</v>
+      </c>
+      <c r="D22">
+        <v>0</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A23" s="1">
+        <v>3</v>
+      </c>
+      <c r="B23">
+        <v>8</v>
+      </c>
+      <c r="C23">
+        <v>1</v>
+      </c>
+      <c r="D23">
+        <v>0</v>
+      </c>
+      <c r="E23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A24" s="1">
+        <v>3</v>
+      </c>
+      <c r="B24">
+        <v>9</v>
+      </c>
+      <c r="C24">
+        <v>0</v>
+      </c>
+      <c r="D24">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A25" s="1">
+        <v>3</v>
+      </c>
+      <c r="B25">
+        <v>10</v>
+      </c>
+      <c r="C25">
+        <v>0</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="E25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>4</v>
+      </c>
+      <c r="B26">
+        <v>1</v>
+      </c>
+      <c r="C26">
+        <v>0</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A27" s="1">
+        <v>4</v>
+      </c>
+      <c r="B27">
+        <v>2</v>
+      </c>
+      <c r="C27">
+        <v>0</v>
+      </c>
+      <c r="D27">
+        <v>0</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A28" s="1">
+        <v>4</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>1</v>
+      </c>
+      <c r="D28">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>5</v>
+      </c>
+      <c r="B29">
+        <v>1</v>
+      </c>
+      <c r="C29">
+        <v>0</v>
+      </c>
+      <c r="D29">
+        <v>0</v>
+      </c>
+      <c r="E29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A30" s="1">
+        <v>5</v>
+      </c>
+      <c r="B30">
+        <v>2</v>
+      </c>
+      <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A31" s="1">
+        <v>5</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31">
+        <v>1</v>
+      </c>
+      <c r="D31">
+        <v>0</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A32" s="1">
+        <v>5</v>
+      </c>
+      <c r="B32">
+        <v>4</v>
+      </c>
+      <c r="C32">
+        <v>0</v>
+      </c>
+      <c r="D32">
+        <v>0</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>6</v>
+      </c>
+      <c r="B33">
+        <v>1</v>
+      </c>
+      <c r="C33">
+        <v>1</v>
+      </c>
+      <c r="D33">
+        <v>0</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A34" s="1">
+        <v>6</v>
+      </c>
+      <c r="B34">
+        <v>2</v>
+      </c>
+      <c r="C34">
+        <v>1</v>
+      </c>
+      <c r="D34">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A35" s="1">
+        <v>6</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35">
+        <v>0</v>
+      </c>
+      <c r="D35">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A36" s="1">
+        <v>6</v>
+      </c>
+      <c r="B36">
+        <v>4</v>
+      </c>
+      <c r="C36">
+        <v>0</v>
+      </c>
+      <c r="D36">
+        <v>0</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A37" s="1">
+        <v>6</v>
+      </c>
+      <c r="B37">
+        <v>5</v>
+      </c>
+      <c r="C37">
+        <v>1</v>
+      </c>
+      <c r="D37">
+        <v>0</v>
+      </c>
+      <c r="E37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A38" s="1">
+        <v>6</v>
+      </c>
+      <c r="B38">
+        <v>6</v>
+      </c>
+      <c r="C38">
+        <v>0</v>
+      </c>
+      <c r="D38">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A39" s="1">
+        <v>6</v>
+      </c>
+      <c r="B39">
+        <v>7</v>
+      </c>
+      <c r="C39">
+        <v>0</v>
+      </c>
+      <c r="D39">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" s="1">
+        <v>6</v>
+      </c>
+      <c r="B40">
+        <v>8</v>
+      </c>
+      <c r="C40">
+        <v>0</v>
+      </c>
+      <c r="D40">
+        <v>0</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>7</v>
+      </c>
+      <c r="B41">
+        <v>1</v>
+      </c>
+      <c r="C41">
+        <v>0</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" s="1">
+        <v>7</v>
+      </c>
+      <c r="B42">
+        <v>2</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" s="1">
+        <v>7</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43">
+        <v>0</v>
+      </c>
+      <c r="D43">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" s="1">
+        <v>7</v>
+      </c>
+      <c r="B44">
+        <v>4</v>
+      </c>
+      <c r="C44">
+        <v>0</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="E44">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" s="1">
+        <v>7</v>
+      </c>
+      <c r="B45">
+        <v>5</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>8</v>
+      </c>
+      <c r="B46">
+        <v>1</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" s="1">
+        <v>8</v>
+      </c>
+      <c r="B47">
+        <v>2</v>
+      </c>
+      <c r="C47">
+        <v>0</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" s="1">
+        <v>8</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>0</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A49" s="1">
+        <v>8</v>
+      </c>
+      <c r="B49">
+        <v>4</v>
+      </c>
+      <c r="C49">
+        <v>0</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A50" s="1">
+        <v>8</v>
+      </c>
+      <c r="B50">
+        <v>5</v>
+      </c>
+      <c r="C50">
+        <v>1</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>9</v>
+      </c>
+      <c r="B51">
+        <v>1</v>
+      </c>
+      <c r="C51">
+        <v>0</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A52" s="1">
+        <v>9</v>
+      </c>
+      <c r="B52">
+        <v>2</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>1</v>
+      </c>
+      <c r="E52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A53" s="1">
+        <v>9</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>0</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A54" s="1">
+        <v>9</v>
+      </c>
+      <c r="B54">
+        <v>4</v>
+      </c>
+      <c r="C54">
+        <v>0</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="E54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A55" s="1">
+        <v>9</v>
+      </c>
+      <c r="B55">
+        <v>5</v>
+      </c>
+      <c r="C55">
+        <v>0</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="E55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A56" s="1">
+        <v>9</v>
+      </c>
+      <c r="B56">
+        <v>6</v>
+      </c>
+      <c r="C56">
+        <v>0</v>
+      </c>
+      <c r="D56">
+        <v>1</v>
+      </c>
+      <c r="E56">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A57" s="1">
+        <v>9</v>
+      </c>
+      <c r="B57">
+        <v>7</v>
+      </c>
+      <c r="C57">
+        <v>1</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="E57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A58">
+        <v>10</v>
+      </c>
+      <c r="B58">
+        <v>1</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
+      <c r="D58">
+        <v>1</v>
+      </c>
+      <c r="E58">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A59" s="1">
+        <v>10</v>
+      </c>
+      <c r="B59">
+        <v>2</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+      <c r="D59">
+        <v>1</v>
+      </c>
+      <c r="E59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A60" s="1">
+        <v>10</v>
+      </c>
+      <c r="B60">
+        <v>3</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+      <c r="D60">
+        <v>1</v>
+      </c>
+      <c r="E60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A61" s="1">
+        <v>10</v>
+      </c>
+      <c r="B61">
+        <v>4</v>
+      </c>
+      <c r="C61">
+        <v>1</v>
+      </c>
+      <c r="D61">
+        <v>1</v>
+      </c>
+      <c r="E61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A62" s="1">
+        <v>10</v>
+      </c>
+      <c r="B62">
+        <v>5</v>
+      </c>
+      <c r="C62">
+        <v>1</v>
+      </c>
+      <c r="D62">
+        <v>1</v>
+      </c>
+      <c r="E62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A63" s="1">
+        <v>10</v>
+      </c>
+      <c r="B63">
+        <v>6</v>
+      </c>
+      <c r="C63">
+        <v>0</v>
+      </c>
+      <c r="D63">
+        <v>1</v>
+      </c>
+      <c r="E63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A64" s="1">
+        <v>10</v>
+      </c>
+      <c r="B64">
+        <v>7</v>
+      </c>
+      <c r="C64">
+        <v>0</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="E64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A65">
+        <v>11</v>
+      </c>
+      <c r="B65">
+        <v>1</v>
+      </c>
+      <c r="C65">
+        <v>0</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="E65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A66" s="1">
+        <v>11</v>
+      </c>
+      <c r="B66">
+        <v>2</v>
+      </c>
+      <c r="C66">
+        <v>0</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="E66">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A67" s="1">
+        <v>11</v>
+      </c>
+      <c r="B67">
+        <v>3</v>
+      </c>
+      <c r="C67">
+        <v>0</v>
+      </c>
+      <c r="D67">
+        <v>1</v>
+      </c>
+      <c r="E67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A68" s="1">
+        <v>11</v>
+      </c>
+      <c r="B68">
+        <v>4</v>
+      </c>
+      <c r="C68">
+        <v>0</v>
+      </c>
+      <c r="D68">
+        <v>1</v>
+      </c>
+      <c r="E68">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A69" s="1">
+        <v>11</v>
+      </c>
+      <c r="B69">
+        <v>5</v>
+      </c>
+      <c r="C69">
+        <v>0</v>
+      </c>
+      <c r="D69">
+        <v>0</v>
+      </c>
+      <c r="E69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A70" s="1">
+        <v>11</v>
+      </c>
+      <c r="B70">
+        <v>6</v>
+      </c>
+      <c r="C70">
+        <v>1</v>
+      </c>
+      <c r="D70">
+        <v>0</v>
+      </c>
+      <c r="E70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A71">
+        <v>12</v>
+      </c>
+      <c r="B71">
+        <v>1</v>
+      </c>
+      <c r="C71">
+        <v>0</v>
+      </c>
+      <c r="D71">
+        <v>0</v>
+      </c>
+      <c r="E71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A72" s="1">
+        <v>12</v>
+      </c>
+      <c r="B72">
+        <v>2</v>
+      </c>
+      <c r="C72">
+        <v>0</v>
+      </c>
+      <c r="D72">
+        <v>1</v>
+      </c>
+      <c r="E72">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A73" s="1">
+        <v>12</v>
+      </c>
+      <c r="B73">
+        <v>3</v>
+      </c>
+      <c r="C73">
+        <v>1</v>
+      </c>
+      <c r="D73">
+        <v>0</v>
+      </c>
+      <c r="E73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A74">
+        <v>13</v>
+      </c>
+      <c r="B74">
+        <v>1</v>
+      </c>
+      <c r="C74">
+        <v>1</v>
+      </c>
+      <c r="D74">
+        <v>0</v>
+      </c>
+      <c r="E74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A75" s="1">
+        <v>13</v>
+      </c>
+      <c r="B75">
+        <v>2</v>
+      </c>
+      <c r="C75">
+        <v>0</v>
+      </c>
+      <c r="D75">
+        <v>1</v>
+      </c>
+      <c r="E75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A76" s="1">
+        <v>13</v>
+      </c>
+      <c r="B76">
+        <v>3</v>
+      </c>
+      <c r="C76">
+        <v>0</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+      <c r="E76">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A77">
+        <v>14</v>
+      </c>
+      <c r="B77">
+        <v>1</v>
+      </c>
+      <c r="C77">
+        <v>0</v>
+      </c>
+      <c r="D77">
+        <v>0</v>
+      </c>
+      <c r="E77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A78" s="1">
+        <v>14</v>
+      </c>
+      <c r="B78">
+        <v>2</v>
+      </c>
+      <c r="C78">
+        <v>0</v>
+      </c>
+      <c r="D78">
+        <v>0</v>
+      </c>
+      <c r="E78">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A79" s="1">
+        <v>14</v>
+      </c>
+      <c r="B79">
+        <v>3</v>
+      </c>
+      <c r="C79">
+        <v>0</v>
+      </c>
+      <c r="D79">
+        <v>0</v>
+      </c>
+      <c r="E79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A80" s="1">
+        <v>14</v>
+      </c>
+      <c r="B80">
+        <v>4</v>
+      </c>
+      <c r="C80">
+        <v>0</v>
+      </c>
+      <c r="D80">
+        <v>0</v>
+      </c>
+      <c r="E80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A81" s="1">
+        <v>14</v>
+      </c>
+      <c r="B81">
+        <v>5</v>
+      </c>
+      <c r="C81">
+        <v>0</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+      <c r="E81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A82" s="1">
+        <v>14</v>
+      </c>
+      <c r="B82">
+        <v>6</v>
+      </c>
+      <c r="C82">
+        <v>1</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+      <c r="E82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A83" s="1">
+        <v>14</v>
+      </c>
+      <c r="B83">
+        <v>7</v>
+      </c>
+      <c r="C83">
+        <v>0</v>
+      </c>
+      <c r="D83">
+        <v>0</v>
+      </c>
+      <c r="E83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A84" s="1">
+        <v>14</v>
+      </c>
+      <c r="B84">
+        <v>8</v>
+      </c>
+      <c r="C84">
+        <v>0</v>
+      </c>
+      <c r="D84">
+        <v>0</v>
+      </c>
+      <c r="E84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A85" s="1">
+        <v>14</v>
+      </c>
+      <c r="B85">
+        <v>9</v>
+      </c>
+      <c r="C85">
+        <v>0</v>
+      </c>
+      <c r="D85">
+        <v>0</v>
+      </c>
+      <c r="E85">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A86" s="1">
+        <v>14</v>
+      </c>
+      <c r="B86">
+        <v>10</v>
+      </c>
+      <c r="C86">
+        <v>0</v>
+      </c>
+      <c r="D86">
+        <v>0</v>
+      </c>
+      <c r="E86">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A87" s="1">
+        <v>14</v>
+      </c>
+      <c r="B87">
+        <v>11</v>
+      </c>
+      <c r="C87">
+        <v>0</v>
+      </c>
+      <c r="D87">
+        <v>0</v>
+      </c>
+      <c r="E87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A88" s="1">
+        <v>14</v>
+      </c>
+      <c r="B88">
+        <v>12</v>
+      </c>
+      <c r="C88">
+        <v>0</v>
+      </c>
+      <c r="D88">
+        <v>0</v>
+      </c>
+      <c r="E88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A89" s="1">
+        <v>14</v>
+      </c>
+      <c r="B89">
+        <v>13</v>
+      </c>
+      <c r="C89">
+        <v>0</v>
+      </c>
+      <c r="D89">
+        <v>1</v>
+      </c>
+      <c r="E89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A90" s="1">
+        <v>14</v>
+      </c>
+      <c r="B90">
+        <v>14</v>
+      </c>
+      <c r="C90">
+        <v>0</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+      <c r="E90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A91">
+        <v>15</v>
+      </c>
+      <c r="B91">
+        <v>1</v>
+      </c>
+      <c r="C91">
+        <v>0</v>
+      </c>
+      <c r="D91">
+        <v>1</v>
+      </c>
+      <c r="E91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A92" s="1">
+        <v>15</v>
+      </c>
+      <c r="B92">
+        <v>2</v>
+      </c>
+      <c r="C92">
+        <v>0</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+      <c r="E92">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A93" s="1">
+        <v>15</v>
+      </c>
+      <c r="B93">
+        <v>3</v>
+      </c>
+      <c r="C93">
+        <v>0</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+      <c r="E93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A94" s="1">
+        <v>15</v>
+      </c>
+      <c r="B94">
+        <v>4</v>
+      </c>
+      <c r="C94">
+        <v>0</v>
+      </c>
+      <c r="D94">
+        <v>0</v>
+      </c>
+      <c r="E94">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A95" s="1">
+        <v>15</v>
+      </c>
+      <c r="B95">
+        <v>5</v>
+      </c>
+      <c r="C95">
+        <v>1</v>
+      </c>
+      <c r="D95">
+        <v>0</v>
+      </c>
+      <c r="E95">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A96">
+        <v>16</v>
+      </c>
+      <c r="B96">
+        <v>1</v>
+      </c>
+      <c r="C96">
+        <v>1</v>
+      </c>
+      <c r="D96">
+        <v>0</v>
+      </c>
+      <c r="E96">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A97" s="1">
+        <v>16</v>
+      </c>
+      <c r="B97">
+        <v>2</v>
+      </c>
+      <c r="C97">
+        <v>1</v>
+      </c>
+      <c r="D97">
+        <v>0</v>
+      </c>
+      <c r="E97">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A98" s="1">
+        <v>16</v>
+      </c>
+      <c r="B98">
+        <v>3</v>
+      </c>
+      <c r="C98">
+        <v>0</v>
+      </c>
+      <c r="D98">
+        <v>0</v>
+      </c>
+      <c r="E98">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A99" s="1">
+        <v>16</v>
+      </c>
+      <c r="B99">
+        <v>4</v>
+      </c>
+      <c r="C99">
+        <v>0</v>
+      </c>
+      <c r="D99">
+        <v>1</v>
+      </c>
+      <c r="E99">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A100" s="1">
+        <v>16</v>
+      </c>
+      <c r="B100">
+        <v>5</v>
+      </c>
+      <c r="C100">
+        <v>0</v>
+      </c>
+      <c r="D100">
+        <v>0</v>
+      </c>
+      <c r="E100">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A101" s="1">
+        <v>16</v>
+      </c>
+      <c r="B101">
+        <v>6</v>
+      </c>
+      <c r="C101">
+        <v>0</v>
+      </c>
+      <c r="D101">
+        <v>0</v>
+      </c>
+      <c r="E101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A102">
+        <v>17</v>
+      </c>
+      <c r="B102">
+        <v>1</v>
+      </c>
+      <c r="C102">
+        <v>1</v>
+      </c>
+      <c r="D102">
+        <v>1</v>
+      </c>
+      <c r="E102">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A103" s="1">
+        <v>17</v>
+      </c>
+      <c r="B103">
+        <v>2</v>
+      </c>
+      <c r="C103">
+        <v>0</v>
+      </c>
+      <c r="D103">
+        <v>0</v>
+      </c>
+      <c r="E103">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A104" s="1">
+        <v>17</v>
+      </c>
+      <c r="B104">
+        <v>3</v>
+      </c>
+      <c r="C104">
+        <v>0</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+      <c r="E104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A105" s="1">
+        <v>17</v>
+      </c>
+      <c r="B105">
+        <v>4</v>
+      </c>
+      <c r="C105">
+        <v>0</v>
+      </c>
+      <c r="D105">
+        <v>0</v>
+      </c>
+      <c r="E105">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A106" s="1">
+        <v>17</v>
+      </c>
+      <c r="B106">
+        <v>5</v>
+      </c>
+      <c r="C106">
+        <v>0</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+      <c r="E106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A107" s="1">
+        <v>17</v>
+      </c>
+      <c r="B107">
+        <v>6</v>
+      </c>
+      <c r="C107">
+        <v>0</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+      <c r="E107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A108">
+        <v>18</v>
+      </c>
+      <c r="B108">
+        <v>1</v>
+      </c>
+      <c r="C108">
+        <v>0</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+      <c r="E108">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A109" s="1">
+        <v>18</v>
+      </c>
+      <c r="B109">
+        <v>2</v>
+      </c>
+      <c r="C109">
+        <v>1</v>
+      </c>
+      <c r="D109">
+        <v>1</v>
+      </c>
+      <c r="E109">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A110" s="1">
+        <v>18</v>
+      </c>
+      <c r="B110">
+        <v>3</v>
+      </c>
+      <c r="C110">
+        <v>0</v>
+      </c>
+      <c r="D110">
+        <v>1</v>
+      </c>
+      <c r="E110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A111" s="1">
+        <v>18</v>
+      </c>
+      <c r="B111">
+        <v>4</v>
+      </c>
+      <c r="C111">
+        <v>0</v>
+      </c>
+      <c r="D111">
+        <v>1</v>
+      </c>
+      <c r="E111">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A112" s="1">
+        <v>18</v>
+      </c>
+      <c r="B112">
+        <v>5</v>
+      </c>
+      <c r="C112">
+        <v>0</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+      <c r="E112">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A113" s="1">
+        <v>18</v>
+      </c>
+      <c r="B113">
+        <v>6</v>
+      </c>
+      <c r="C113">
+        <v>1</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+      <c r="E113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A114" s="1">
+        <v>18</v>
+      </c>
+      <c r="B114">
+        <v>7</v>
+      </c>
+      <c r="C114">
+        <v>1</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+      <c r="E114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A115" s="1">
+        <v>18</v>
+      </c>
+      <c r="B115">
+        <v>8</v>
+      </c>
+      <c r="C115">
+        <v>0</v>
+      </c>
+      <c r="D115">
+        <v>0</v>
+      </c>
+      <c r="E115">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A116" s="1">
+        <v>18</v>
+      </c>
+      <c r="B116">
+        <v>9</v>
+      </c>
+      <c r="C116">
+        <v>0</v>
+      </c>
+      <c r="D116">
+        <v>0</v>
+      </c>
+      <c r="E116">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Explanation xmlns="852793cc-10af-4c56-90ee-405dd9e420a3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8534,17 +10800,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Explanation xmlns="852793cc-10af-4c56-90ee-405dd9e420a3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B99141-A835-4B42-8F06-1A61E0E287ED}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE4C6F5-600E-4EB6-AB93-607B9AC5B2A4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="852793cc-10af-4c56-90ee-405dd9e420a3"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -8569,11 +10838,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE4C6F5-600E-4EB6-AB93-607B9AC5B2A4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B99141-A835-4B42-8F06-1A61E0E287ED}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="852793cc-10af-4c56-90ee-405dd9e420a3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Added flag to TemplateXLSX for inhibitor value override.
</commit_message>
<xml_diff>
--- a/AdapQuestBackend/data/templates/adaptive.questionnaire.template.xlsx
+++ b/AdapQuestBackend/data/templates/adaptive.questionnaire.template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Development\adaptive\adapquest\AdapQuestBackend\data\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55C55119-E18A-4CC7-9AAC-511B33BC686B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53A094B-2AE1-4D6A-862E-5BF59D7E1833}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15990" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Settings" sheetId="11" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="189">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="237" uniqueCount="191">
   <si>
     <t>Mandatory</t>
   </si>
@@ -604,6 +604,12 @@
   </si>
   <si>
     <t>Profiles</t>
+  </si>
+  <si>
+    <t>INHIBITOR_DEFAULT_VALUE</t>
+  </si>
+  <si>
+    <t>INHIBITOR_OVERRIDE_VALUE_WITH_DEFAULT</t>
   </si>
 </sst>
 </file>
@@ -1006,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9A944510-FF7A-456D-8D81-52A411BFF42E}">
-  <dimension ref="A1:B22"/>
+  <dimension ref="A1:B24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1051,59 +1057,59 @@
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="2" t="s">
+      <c r="A5" t="s">
+        <v>190</v>
+      </c>
+      <c r="B5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+    <row r="8" spans="1:2" s="1" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>152</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B8" s="2" t="s">
         <v>168</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>153</v>
-      </c>
-      <c r="B7" s="3"/>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>154</v>
-      </c>
-      <c r="B8">
-        <v>3600</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>155</v>
-      </c>
+        <v>153</v>
+      </c>
+      <c r="B9" s="3"/>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>156</v>
-      </c>
-      <c r="B10" t="b">
-        <v>1</v>
+        <v>154</v>
+      </c>
+      <c r="B10">
+        <v>3600</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>157</v>
-      </c>
-      <c r="B11" t="b">
-        <v>0</v>
+        <v>155</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="B12" t="b">
         <v>1</v>
@@ -1111,86 +1117,103 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B13" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="B14" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>161</v>
-      </c>
-      <c r="B15">
-        <v>0</v>
+        <v>159</v>
+      </c>
+      <c r="B15" t="b">
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16">
-        <v>1000</v>
+        <v>160</v>
+      </c>
+      <c r="B16" t="b">
+        <v>0</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>26</v>
+        <v>161</v>
       </c>
       <c r="B17">
-        <v>18</v>
+        <v>0</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B18">
-        <v>18</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="B19">
-        <v>0.1</v>
+        <v>18</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="B20">
-        <v>0.25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B21">
-        <v>1</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
+        <v>165</v>
+      </c>
+      <c r="B22">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A23" t="s">
+        <v>166</v>
+      </c>
+      <c r="B23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A24" t="s">
         <v>167</v>
       </c>
-      <c r="B22">
+      <c r="B24">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -8595,7 +8618,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A7DD315C-5019-4FDD-A7E5-B0550B9F67F5}">
   <dimension ref="A1:E116"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
@@ -10575,6 +10598,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x0101001993BA935880B747A0EBD22E55DF1701" ma:contentTypeVersion="14" ma:contentTypeDescription="Creare un nuovo documento." ma:contentTypeScope="" ma:versionID="80da22eab6347bd8afd3fcbce4f6dc5a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="852793cc-10af-4c56-90ee-405dd9e420a3" xmlns:ns3="e9ad1ca7-101c-4f77-8d13-c4641e513550" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="db6456f859ea161d1f2465791bd09b5e" ns2:_="" ns3:_="">
     <xsd:import namespace="852793cc-10af-4c56-90ee-405dd9e420a3"/>
@@ -10799,15 +10831,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4DE4C6F5-600E-4EB6-AB93-607B9AC5B2A4}">
   <ds:schemaRefs>
@@ -10819,6 +10842,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B99141-A835-4B42-8F06-1A61E0E287ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1834EA7F-0E79-4F99-862A-1B8D20441A61}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -10835,12 +10866,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C5B99141-A835-4B42-8F06-1A61E0E287ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>